<commit_message>
Fixed scripts for the server
</commit_message>
<xml_diff>
--- a/output_partially_covered_generated.xlsx
+++ b/output_partially_covered_generated.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Distance</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Content</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Distance</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">

</xml_diff>